<commit_message>
Add refined vertical treebank
</commit_message>
<xml_diff>
--- a/Random Sample/Annotated/Eval2.xlsx
+++ b/Random Sample/Annotated/Eval2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristopherkyle/Desktop/Programming/GitHub/LCR-ADS-Lab/ASC-Treebank/ASC-Treebank/Random Sample/Annotated/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D183CB-329D-4042-8D03-BAE2C0E55921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FB70FF-0C68-CC4B-91AE-ACE195164004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="anno2" sheetId="1" r:id="rId1"/>
@@ -7096,8 +7096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1750"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L272" sqref="L272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>